<commit_message>
add color borders to regular orders
</commit_message>
<xml_diff>
--- a/rakuten/點數-冷凍.xlsx
+++ b/rakuten/點數-冷凍.xlsx
@@ -11317,7 +11317,7 @@
     <col customWidth="1" max="6" min="6" width="12"/>
     <col customWidth="1" max="7" min="7" width="13"/>
     <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="40"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
     <col customWidth="1" max="10" min="10" width="40"/>
     <col customWidth="1" max="11" min="11" width="6"/>
     <col customWidth="1" max="12" min="12" width="6"/>
@@ -73400,7 +73400,7 @@
     <col customWidth="1" max="6" min="6" width="12"/>
     <col customWidth="1" max="7" min="7" width="13"/>
     <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="40"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
     <col customWidth="1" max="10" min="10" width="40"/>
     <col customWidth="1" max="11" min="11" width="6"/>
     <col customWidth="1" max="12" min="12" width="6"/>
@@ -81184,7 +81184,7 @@
     <col customWidth="1" max="6" min="6" width="12"/>
     <col customWidth="1" max="7" min="7" width="13"/>
     <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="40"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
     <col customWidth="1" max="10" min="10" width="40"/>
     <col customWidth="1" max="11" min="11" width="6"/>
     <col customWidth="1" max="12" min="12" width="6"/>
@@ -85749,7 +85749,7 @@
     <col customWidth="1" max="6" min="6" width="12"/>
     <col customWidth="1" max="7" min="7" width="13"/>
     <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="40"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
     <col customWidth="1" max="10" min="10" width="40"/>
     <col customWidth="1" max="11" min="11" width="6"/>
     <col customWidth="1" max="12" min="12" width="6"/>
@@ -90052,7 +90052,7 @@
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="13"/>
     <col customWidth="1" max="8" min="8" width="13"/>
-    <col customWidth="1" max="9" min="9" width="40"/>
+    <col customWidth="1" max="9" min="9" width="20"/>
     <col customWidth="1" max="10" min="10" width="40"/>
     <col customWidth="1" max="11" min="11" width="6"/>
     <col customWidth="1" max="12" min="12" width="6"/>

</xml_diff>